<commit_message>
Add prosumer sensitivity outputs
</commit_message>
<xml_diff>
--- a/Outputs/1. Budget/Grid Search/Output Files/250000/Output_0_1.xlsx
+++ b/Outputs/1. Budget/Grid Search/Output Files/250000/Output_0_1.xlsx
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-64583.49291780668</v>
+        <v>-64583.49291780667</v>
       </c>
     </row>
     <row r="7">
@@ -26335,7 +26335,7 @@
         <v>5375.370276572319</v>
       </c>
       <c r="J2" t="n">
-        <v>5375.370276572321</v>
+        <v>5375.370276572319</v>
       </c>
       <c r="K2" t="n">
         <v>5375.370276572319</v>
@@ -26350,7 +26350,7 @@
         <v>5375.370276572321</v>
       </c>
       <c r="O2" t="n">
-        <v>5375.370276572321</v>
+        <v>5375.37027657232</v>
       </c>
       <c r="P2" t="n">
         <v>5375.370276572319</v>
@@ -26415,49 +26415,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="C4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="D4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="E4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="F4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="G4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="H4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="I4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="J4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="K4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="L4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="M4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="N4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="O4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
       <c r="P4" t="n">
-        <v>2099.754014286062</v>
+        <v>2099.754014286063</v>
       </c>
     </row>
     <row r="5">
@@ -26543,7 +26543,7 @@
         <v>3275.616262286257</v>
       </c>
       <c r="J6" t="n">
-        <v>3275.616262286259</v>
+        <v>3275.616262286257</v>
       </c>
       <c r="K6" t="n">
         <v>3275.616262286257</v>
@@ -26555,10 +26555,10 @@
         <v>3275.616262286257</v>
       </c>
       <c r="N6" t="n">
-        <v>3275.616262286259</v>
+        <v>3275.616262286258</v>
       </c>
       <c r="O6" t="n">
-        <v>3275.616262286259</v>
+        <v>3275.616262286258</v>
       </c>
       <c r="P6" t="n">
         <v>3275.616262286257</v>

</xml_diff>